<commit_message>
Adding FreezePane for Header
</commit_message>
<xml_diff>
--- a/Suspicion.xlsx
+++ b/Suspicion.xlsx
@@ -13543,7 +13543,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E4490"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" tabSelected="true">
+      <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>

</xml_diff>